<commit_message>
Stereotype aan shapes gehangen ipv classes
</commit_message>
<xml_diff>
--- a/catalogusdata/Concepten/Regressietest/xls/Uploadcontrole.xlsx
+++ b/catalogusdata/Concepten/Regressietest/xls/Uploadcontrole.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="156">
   <si>
     <t>tabblad</t>
   </si>
@@ -487,6 +487,12 @@
   </si>
   <si>
     <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{engerdan}</t>
+  </si>
+  <si>
+    <t>dctype</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/dcmitype/{klasse}</t>
   </si>
 </sst>
 </file>
@@ -895,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,11 +912,12 @@
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,41 +928,44 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -965,14 +975,14 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -982,409 +992,442 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
       <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>89</v>
       </c>
       <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
       <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>141</v>
-      </c>
-      <c r="B30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>141</v>
       </c>
       <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="2"/>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D6" r:id="rId2" location="{eigenschap}"/>
-    <hyperlink ref="D12" r:id="rId3" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
-    <hyperlink ref="D13" r:id="rId4" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
-    <hyperlink ref="D14" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
-    <hyperlink ref="D15" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
-    <hyperlink ref="D16" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
-    <hyperlink ref="D22" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D23" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="D9" r:id="rId10" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="D7" r:id="rId11" location="{eigenschap}"/>
-    <hyperlink ref="D2" r:id="rId12" location="{klasse}"/>
-    <hyperlink ref="D11" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D28" r:id="rId14"/>
-    <hyperlink ref="D27" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D25" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
-    <hyperlink ref="D26" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D30" r:id="rId18"/>
-    <hyperlink ref="D31" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="D8" r:id="rId20"/>
-    <hyperlink ref="D10" r:id="rId21"/>
-    <hyperlink ref="D24" r:id="rId22"/>
-    <hyperlink ref="D17" r:id="rId23"/>
-    <hyperlink ref="D18" r:id="rId24"/>
-    <hyperlink ref="D19" r:id="rId25"/>
-    <hyperlink ref="D20" r:id="rId26"/>
-    <hyperlink ref="D21" r:id="rId27"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2" location="{eigenschap}"/>
+    <hyperlink ref="E13" r:id="rId3" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
+    <hyperlink ref="E14" r:id="rId4" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
+    <hyperlink ref="E15" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
+    <hyperlink ref="E16" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
+    <hyperlink ref="E17" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
+    <hyperlink ref="E23" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="E24" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="E10" r:id="rId10" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="E8" r:id="rId11" location="{eigenschap}"/>
+    <hyperlink ref="E2" r:id="rId12" location="{klasse}"/>
+    <hyperlink ref="E12" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="E29" r:id="rId14"/>
+    <hyperlink ref="E28" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="E26" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
+    <hyperlink ref="E27" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="E31" r:id="rId18"/>
+    <hyperlink ref="E32" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="E9" r:id="rId20"/>
+    <hyperlink ref="E11" r:id="rId21"/>
+    <hyperlink ref="E25" r:id="rId22"/>
+    <hyperlink ref="E18" r:id="rId23"/>
+    <hyperlink ref="E19" r:id="rId24"/>
+    <hyperlink ref="E20" r:id="rId25"/>
+    <hyperlink ref="E21" r:id="rId26"/>
+    <hyperlink ref="E22" r:id="rId27"/>
+    <hyperlink ref="E3" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 
@@ -1392,7 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
@@ -2823,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,9 +2904,6 @@
       <c r="A2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
       <c r="C2" s="5" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Revert of accidental commit
</commit_message>
<xml_diff>
--- a/catalogusdata/Concepten/Regressietest/xls/Uploadcontrole.xlsx
+++ b/catalogusdata/Concepten/Regressietest/xls/Uploadcontrole.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="154">
   <si>
     <t>tabblad</t>
   </si>
@@ -487,12 +487,6 @@
   </si>
   <si>
     <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{engerdan}</t>
-  </si>
-  <si>
-    <t>dctype</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/dcmitype/{klasse}</t>
   </si>
 </sst>
 </file>
@@ -901,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,12 +906,11 @@
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,44 +921,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -975,14 +965,14 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -992,442 +982,409 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>141</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="2"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2" location="{eigenschap}"/>
-    <hyperlink ref="E13" r:id="rId3" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
-    <hyperlink ref="E14" r:id="rId4" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
-    <hyperlink ref="E15" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
-    <hyperlink ref="E16" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
-    <hyperlink ref="E17" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
-    <hyperlink ref="E23" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="E24" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="E10" r:id="rId10" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="E8" r:id="rId11" location="{eigenschap}"/>
-    <hyperlink ref="E2" r:id="rId12" location="{klasse}"/>
-    <hyperlink ref="E12" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="E29" r:id="rId14"/>
-    <hyperlink ref="E28" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="E26" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
-    <hyperlink ref="E27" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="E31" r:id="rId18"/>
-    <hyperlink ref="E32" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
-    <hyperlink ref="E9" r:id="rId20"/>
-    <hyperlink ref="E11" r:id="rId21"/>
-    <hyperlink ref="E25" r:id="rId22"/>
-    <hyperlink ref="E18" r:id="rId23"/>
-    <hyperlink ref="E19" r:id="rId24"/>
-    <hyperlink ref="E20" r:id="rId25"/>
-    <hyperlink ref="E21" r:id="rId26"/>
-    <hyperlink ref="E22" r:id="rId27"/>
-    <hyperlink ref="E3" r:id="rId28"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2" location="{eigenschap}"/>
+    <hyperlink ref="D12" r:id="rId3" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
+    <hyperlink ref="D13" r:id="rId4" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
+    <hyperlink ref="D14" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
+    <hyperlink ref="D15" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
+    <hyperlink ref="D16" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
+    <hyperlink ref="D22" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D23" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D9" r:id="rId10" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D7" r:id="rId11" location="{eigenschap}"/>
+    <hyperlink ref="D2" r:id="rId12" location="{klasse}"/>
+    <hyperlink ref="D11" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="D28" r:id="rId14"/>
+    <hyperlink ref="D27" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="D25" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
+    <hyperlink ref="D26" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D30" r:id="rId18"/>
+    <hyperlink ref="D31" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="D10" r:id="rId21"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D17" r:id="rId23"/>
+    <hyperlink ref="D18" r:id="rId24"/>
+    <hyperlink ref="D19" r:id="rId25"/>
+    <hyperlink ref="D20" r:id="rId26"/>
+    <hyperlink ref="D21" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -1435,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
@@ -2866,8 +2823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,6 +2861,9 @@
       <c r="A2" t="s">
         <v>114</v>
       </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Eerste versie voorbeeldbestand data waardelijsten
</commit_message>
<xml_diff>
--- a/catalogusdata/Concepten/Regressietest/xls/Uploadcontrole.xlsx
+++ b/catalogusdata/Concepten/Regressietest/xls/Uploadcontrole.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="4755" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="4755" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="144">
   <si>
     <t>tabblad</t>
   </si>
@@ -429,12 +429,6 @@
   </si>
   <si>
     <t>Standaard beesten</t>
-  </si>
-  <si>
-    <t>Monster</t>
-  </si>
-  <si>
-    <t>Toeleidingsbegrippen</t>
   </si>
   <si>
     <t>http://{source}</t>
@@ -1034,7 +1028,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E8" t="s">
         <v>120</v>
@@ -1062,7 +1056,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,7 +1133,7 @@
         <v>119</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1144,7 @@
         <v>122</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,7 +1155,7 @@
         <v>125</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,7 +1166,7 @@
         <v>128</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,7 +1177,7 @@
         <v>131</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,7 +1213,7 @@
         <v>27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,7 +1274,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2459,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,19 +2515,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" t="s">
-        <v>136</v>
-      </c>
       <c r="E4" s="10"/>
-      <c r="F4" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="10"/>
@@ -2633,7 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2684,7 +2666,7 @@
         <v>42552</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>